<commit_message>
Added 'location' endpoints to REST API interface
</commit_message>
<xml_diff>
--- a/DEMO/Maritza/demo-3/SiPM_bundle.xlsx
+++ b/DEMO/Maritza/demo-3/SiPM_bundle.xlsx
@@ -33,7 +33,7 @@
     <t xml:space="preserve">SiPM_Strip_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Test-008</t>
+    <t xml:space="preserve">Test-010</t>
   </si>
   <si>
     <t xml:space="preserve">External_ID</t>
@@ -781,7 +781,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -825,7 +825,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -895,7 +895,7 @@
       </c>
       <c r="E2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
@@ -911,7 +911,7 @@
       </c>
       <c r="J2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
@@ -996,7 +996,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>34</v>
@@ -1038,7 +1038,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>34</v>
@@ -1080,7 +1080,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>34</v>
@@ -1122,7 +1122,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>34</v>
@@ -1164,7 +1164,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
@@ -1206,7 +1206,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
@@ -1328,7 +1328,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>47</v>
@@ -1379,7 +1379,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>47</v>
@@ -1430,7 +1430,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>47</v>
@@ -1481,7 +1481,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>47</v>
@@ -1532,7 +1532,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>47</v>
@@ -1583,7 +1583,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>47</v>
@@ -1634,7 +1634,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>67</v>
@@ -1679,7 +1679,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
@@ -1724,7 +1724,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>67</v>
@@ -1769,7 +1769,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>67</v>
@@ -1814,7 +1814,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>67</v>
@@ -1859,7 +1859,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>67</v>
@@ -1904,7 +1904,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>86</v>
@@ -1955,7 +1955,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
@@ -2006,7 +2006,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>86</v>
@@ -2057,7 +2057,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>86</v>
@@ -2108,7 +2108,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>86</v>
@@ -2159,7 +2159,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
@@ -2210,7 +2210,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>105</v>
@@ -2255,7 +2255,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>105</v>
@@ -2300,7 +2300,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>105</v>
@@ -2345,7 +2345,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>105</v>
@@ -2390,7 +2390,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>105</v>
@@ -2435,7 +2435,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>105</v>
@@ -2480,7 +2480,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>124</v>
@@ -2531,7 +2531,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>124</v>
@@ -2582,7 +2582,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>124</v>
@@ -2633,7 +2633,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>124</v>
@@ -2684,7 +2684,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>124</v>
@@ -2735,7 +2735,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>124</v>
@@ -2786,7 +2786,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>144</v>
@@ -2831,7 +2831,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>144</v>
@@ -2876,7 +2876,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>144</v>
@@ -2921,7 +2921,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>144</v>
@@ -2966,7 +2966,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>144</v>
@@ -3011,7 +3011,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>144</v>
@@ -3136,7 +3136,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>168</v>
@@ -3190,7 +3190,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>168</v>
@@ -3244,7 +3244,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>168</v>
@@ -3298,7 +3298,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>168</v>
@@ -3352,7 +3352,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>168</v>
@@ -3406,7 +3406,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>168</v>
@@ -3538,7 +3538,7 @@
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>47</v>
@@ -3580,7 +3580,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>47</v>
@@ -3622,7 +3622,7 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>47</v>
@@ -3664,7 +3664,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>47</v>
@@ -3706,7 +3706,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>47</v>
@@ -3748,7 +3748,7 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>47</v>
@@ -3790,7 +3790,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>67</v>
@@ -3832,7 +3832,7 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
@@ -3874,7 +3874,7 @@
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>67</v>
@@ -3916,7 +3916,7 @@
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>67</v>
@@ -3958,7 +3958,7 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>67</v>
@@ -4000,7 +4000,7 @@
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>67</v>
@@ -4042,7 +4042,7 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>86</v>
@@ -4084,7 +4084,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
@@ -4126,7 +4126,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>86</v>
@@ -4168,7 +4168,7 @@
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>86</v>
@@ -4210,7 +4210,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>86</v>
@@ -4252,7 +4252,7 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
@@ -4294,7 +4294,7 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>105</v>
@@ -4336,7 +4336,7 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>105</v>
@@ -4378,7 +4378,7 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>105</v>
@@ -4420,7 +4420,7 @@
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>105</v>
@@ -4462,7 +4462,7 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>105</v>
@@ -4504,7 +4504,7 @@
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>105</v>
@@ -4546,7 +4546,7 @@
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>124</v>
@@ -4588,7 +4588,7 @@
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>124</v>
@@ -4630,7 +4630,7 @@
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>124</v>
@@ -4672,7 +4672,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>124</v>
@@ -4714,7 +4714,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>124</v>
@@ -4756,7 +4756,7 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>124</v>
@@ -4798,7 +4798,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>144</v>
@@ -4840,7 +4840,7 @@
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>144</v>
@@ -4882,7 +4882,7 @@
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>144</v>
@@ -4924,7 +4924,7 @@
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>144</v>
@@ -4966,7 +4966,7 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>144</v>
@@ -5008,7 +5008,7 @@
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>144</v>
@@ -5050,7 +5050,7 @@
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>34</v>
@@ -5092,7 +5092,7 @@
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>34</v>
@@ -5134,7 +5134,7 @@
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>34</v>
@@ -5176,7 +5176,7 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>34</v>
@@ -5218,7 +5218,7 @@
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>34</v>
@@ -5260,7 +5260,7 @@
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="str">
         <f aca="false">Instructions!$B$3</f>
-        <v>Test-008</v>
+        <v>Test-010</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>34</v>

</xml_diff>